<commit_message>
initial updates to requirements
</commit_message>
<xml_diff>
--- a/lib/davinci_crd_test_kit/requirements/hl7.fhir.us.davinci-crd_2.0.1_requirements.xlsx
+++ b/lib/davinci_crd_test_kit/requirements/hl7.fhir.us.davinci-crd_2.0.1_requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/davinci-crd-test-kit/lib/davinci_crd_test_kit/requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlnaden/GlenViewAssociates/Inferno/source/davinci-crd-test-kit/lib/davinci_crd_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE216CD-C581-0E41-8635-FE85C4BEB01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B452F66-A00F-D34F-886A-0264B992CB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="5620" windowWidth="34560" windowHeight="20180" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="3340" yWindow="760" windowWidth="34260" windowHeight="21260" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="476">
   <si>
     <r>
       <rPr>
@@ -1826,12 +1826,6 @@
     <t>This  [[encounter-discharge](https://cds-hooks.hl7.org/hooks/encounter-discharge/STU1/encounter-discharge/)] hook would generally be specific to an in-patient encounter and would fire when a provider is performing the discharge process within the CRD Client.</t>
   </si>
   <si>
-    <t>[In response to an [encounter-discharge](https://cds-hooks.hl7.org/hooks/encounter-discharge/STU1/encounter-discharge/) hook call, [clients should] Verify that documentation requirements for the services performed have been met to ensure the services provided can be reimbursed</t>
-  </si>
-  <si>
-    <t>[In response to an [encounter-discharge](https://cds-hooks.hl7.org/hooks/encounter-discharge/STU1/encounter-discharge/) hook call, [clients should] Ensure that required follow-up planning is complete and appropriate transfer of care has been arranged, particularly for accountable care models</t>
-  </si>
-  <si>
     <t>[for the [encounter-discharge](https://cds-hooks.hl7.org/hooks/encounter-discharge/STU1/encounter-discharge/) hook] The profiles expected to be used for the resources resolved to by the userId … are … [profile-practitioner](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-practitioner.html) [or] [us-core-practitionerrole](http://hl7.org/fhir/us/core/STU3.1.1/StructureDefinition-us-core-practitionerrole.html)</t>
   </si>
   <si>
@@ -1862,67 +1856,10 @@
     <t>https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-select</t>
   </si>
   <si>
-    <t xml:space="preserve">[Servers SHALL support] version 1.0 of the [[order-select](https://cds-hooks.hl7.org/hooks/order-select/2023SepSTU1Ballot/order-select/)] Hook  [([published v1.0 link](https://cds-hooks.hl7.org/hooks/order-select/STU1/order-select/))] </t>
-  </si>
-  <si>
     <t xml:space="preserve"> conditional on supporting the indicated hook.</t>
   </si>
   <si>
-    <t xml:space="preserve">[Clients SHALL support] version 1.0 of the [[order-select](https://cds-hooks.hl7.org/hooks/order-select/2023SepSTU1Ballot/order-select/)] Hook [([published v1.0 link](https://cds-hooks.hl7.org/hooks/order-select/STU1/order-select/))] </t>
-  </si>
-  <si>
-    <t>Coverage requirements [returned from the [order-select hook](https://cds-hooks.hl7.org/hooks/order-select/STU1/order-select/)] SHOULD be limited only to those resources that are included in the `selections` context</t>
-  </si>
-  <si>
-    <t>the content of other [resources that are not included in the `selections` context] resources  [[for the order-select hook](https://cds-hooks.hl7.org/hooks/order-select/STU1/order-select/)] SHOULD also be considered before making recommendations about what additional actions are necessary. (I.e. don’t recommend an action if there’s already a draft order to perform that action.)</t>
-  </si>
-  <si>
-    <t>[For the [order-select](https://cds-hooks.hl7.org/hooks/order-select/STU1/order-select/) hook] the profiles expected to be used for the resources resolved to by the `patientId` [are] [profile-patient](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-patient.html)</t>
-  </si>
-  <si>
-    <t>[For the [order-select](https://cds-hooks.hl7.org/hooks/order-select/STU1/order-select/) hook] the profiles expected to be used for the resources resolved to by the … `encounterId` [are] [profile-encounter](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-encounter.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[for the [order-select](https://cds-hooks.hl7.org/hooks/order-select/STU1/order-select/) hook] The profiles expected to be used for the resources resolved to by the ... `draftOrders` context element [are] [profile-devicerequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-devicerequest.html), [profile-medicationrequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-medicationrequest.html), [profile-nutritionorder](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-nutritionorder.html), [profile-visionprescription](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-visionprescription.html), [and] [profile-servicerequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-servicerequest.html) </t>
-  </si>
-  <si>
-    <t>While this [order-select](https://cds-hooks.hl7.org/hooks/order-select/STU1/order-select/)] hook does not explicitly list PractitionerRole [([us-core-practitionerrole](http://hl7.org/fhir/us/core/STU3.1.1/StructureDefinition-us-core-practitionerrole.html)) in addition to  [profile-practitioner](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-practitioner.html)] as an expected resource type for userId, it is not prohibited and is included to allow linking the user to a Practitioner in a specific role acting on behalf of a specific Organization.</t>
-  </si>
-  <si>
-    <t>This [[order-select](https://cds-hooks.hl7.org/hooks/order-select/STU1/order-select/)] hook MAY be used in scenarios that don’t involve creating a true order</t>
-  </si>
-  <si>
     <t>https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-sign</t>
-  </si>
-  <si>
-    <t>[Servers SHALL support] version 1.0 of the [[order-sign](https://cds-hooks.org/hooks/order-sign/2020May/order-sign)] Hook. [([published v1.0 link](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/))]</t>
-  </si>
-  <si>
-    <t>[Clients SHALL support] version 1.0 of the [[order-sign](https://cds-hooks.org/hooks/order-sign/2020May/order-sign)] Hook [([published v1.0 link](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/))]</t>
-  </si>
-  <si>
-    <t>[[For the order-sign hook](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/)] It’s appropriate to provide warnings if there is insufficient information to determine coverage requirements.</t>
-  </si>
-  <si>
-    <t>Use and profiles for [order-select](https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-select) also apply to [order-sign](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/) [including: the profiles expected to be used for the resources resolved to by the `patientId`are [profile-patient](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-patient.html)]</t>
-  </si>
-  <si>
-    <t>Use and profiles for [order-select](https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-select) also apply to [order-sign](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/) [including: the profiles expected to be used for the resources resolved to by the … `encounterId` are [profile-encounter](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-encounter.html)]</t>
-  </si>
-  <si>
-    <t>Use and profiles for [order-select](https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-select) also apply to [order-sign](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/) [including: The profiles expected to be used for the resources resolved to by the ... `draftOrders` context element [are] [profile-devicerequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-devicerequest.html), [profile-medicationrequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-medicationrequest.html), [profile-nutritionorder](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-nutritionorder.html), [profile-visionprescription](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-visionprescription.html),  [profile-servicerequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-servicerequest.html)]</t>
-  </si>
-  <si>
-    <t>Use and profiles for [order-select](https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-select) also apply to [order-sign](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/) [including: while this hook does not explicitly list PractitionerRole [([us-core-practitionerrole](http://hl7.org/fhir/us/core/STU3.1.1/StructureDefinition-us-core-practitionerrole.html)) in addition to  [profile-practitioner](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-practitioner.html)] as an expected resource type for userId, it is not prohibited and is included to allow linking the user to a Practitioner in a specific role acting on behalf of a specific Organization.]</t>
-  </si>
-  <si>
-    <t>CRD Servers MAY use this [[order-sign hook](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/)] hook as a basis for associating a patient with a particular practitioner from a payer attribution perspective.</t>
-  </si>
-  <si>
-    <t>CRD clients ... SHALL, at minimum, support returning … processing the Coverage Information system action for all invocations of this [[order-sign hook](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/)] hook.</t>
-  </si>
-  <si>
-    <t>CRD... servers SHALL, at minimum, support... processing the Coverage Information system action for all invocations of this [[order-sign hook](https://cds-hooks.hl7.org/hooks/order-sign/STU1/order-sign/)] hook.</t>
   </si>
   <si>
     <t>https://hl7.org/fhir/us/davinci-crd/STU2/cards.html#cards-profiles</t>
@@ -2982,6 +2919,147 @@
   </si>
   <si>
     <t>this is text describing and the requirement is actually in requirement 135, so marked as DEPRECATED.</t>
+  </si>
+  <si>
+    <t>conditional on requirement 20: if clients allow users to continue their workflow before long-running CRD results return, then this is a requirement.</t>
+  </si>
+  <si>
+    <t>[Clients SHALL support] version 1.1 of the [[order-sign](https://cds-hooks.org/hooks/order-sign/2020May/order-sign)] Hook [([published v1.0 link (v1.1.0 in the change log)](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html))]</t>
+  </si>
+  <si>
+    <t>[Servers SHALL support] version 1.1 of the [[order-sign](https://cds-hooks.org/hooks/order-sign/2020May/order-sign)] Hook [([published v1.0 link (v1.1.0 in the change log)](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html))]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Servers SHALL support] version 1.0 of the [[order-select](https://cds-hooks.hl7.org/hooks/order-select/2023SepSTU1Ballot/order-select/)] Hook  [([published v1.0 link](https://cds-hooks.hl7.org/hooks/order-select.html))] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Clients SHALL support] version 1.0 of the [[order-select](https://cds-hooks.hl7.org/hooks/order-select/2023SepSTU1Ballot/order-select/)] Hook [([published v1.0 link](https://cds-hooks.hl7.org/hooks/order-select.html))] </t>
+  </si>
+  <si>
+    <t>Coverage requirements [returned from the [order-select hook](https://cds-hooks.hl7.org/hooks/order-select.html)] SHOULD be limited only to those resources that are included in the `selections` context</t>
+  </si>
+  <si>
+    <t>the content of other [resources that are not included in the `selections` context] resources  [[for the order-select hook](https://cds-hooks.hl7.org/hooks/order-select.html)] SHOULD also be considered before making recommendations about what additional actions are necessary. (I.e. don’t recommend an action if there’s already a draft order to perform that action.)</t>
+  </si>
+  <si>
+    <t>[For the [order-select](https://cds-hooks.hl7.org/hooks/order-select.html) hook] the profiles expected to be used for the resources resolved to by the `patientId` [are] [profile-patient](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-patient.html)</t>
+  </si>
+  <si>
+    <t>[For the [order-select](https://cds-hooks.hl7.org/hooks/order-select.html) hook] the profiles expected to be used for the resources resolved to by the … `encounterId` [are] [profile-encounter](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-encounter.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[for the [order-select](https://cds-hooks.hl7.org/hooks/order-select.html) hook] The profiles expected to be used for the resources resolved to by the ... `draftOrders` context element [are] [profile-devicerequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-devicerequest.html), [profile-medicationrequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-medicationrequest.html), [profile-nutritionorder](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-nutritionorder.html), [profile-visionprescription](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-visionprescription.html), [and] [profile-servicerequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-servicerequest.html) </t>
+  </si>
+  <si>
+    <t>While this [order-select](https://cds-hooks.hl7.org/hooks/order-select.html)] hook does not explicitly list PractitionerRole [([us-core-practitionerrole](http://hl7.org/fhir/us/core/STU3.1.1/StructureDefinition-us-core-practitionerrole.html)) in addition to  [profile-practitioner](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-practitioner.html)] as an expected resource type for userId, it is not prohibited and is included to allow linking the user to a Practitioner in a specific role acting on behalf of a specific Organization.</t>
+  </si>
+  <si>
+    <t>This [[order-select](https://cds-hooks.hl7.org/hooks/order-select.html)] hook MAY be used in scenarios that don’t involve creating a true order</t>
+  </si>
+  <si>
+    <t>[[For the order-sign hook](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html)] It’s appropriate to provide warnings if there is insufficient information to determine coverage requirements.</t>
+  </si>
+  <si>
+    <t>CRD Servers MAY use this [[order-sign hook](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html)] hook as a basis for associating a patient with a particular practitioner from a payer attribution perspective.</t>
+  </si>
+  <si>
+    <t>CRD clients ... SHALL, at minimum, support … processing the Coverage Information system action for all invocations of this [[order-sign hook](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html)] hook.</t>
+  </si>
+  <si>
+    <t>CRD... servers SHALL, at minimum, support returning ... the Coverage Information system action for all invocations of this [[order-sign hook](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html)] hook.</t>
+  </si>
+  <si>
+    <t>Use and profiles for [order-select](https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-select) also apply to `order-sign` [([link](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html)) including: the profiles expected to be used for the resources resolved to by the `patientId`are [profile-patient](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-patient.html)]</t>
+  </si>
+  <si>
+    <t>Use and profiles for [order-select](https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-select) also apply to `order-sign` [([link](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html)) including: the profiles expected to be used for the resources resolved to by the … `encounterId` are [profile-encounter](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-encounter.html)]</t>
+  </si>
+  <si>
+    <t>Use and profiles for [order-select](https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-select) also apply to `order-sign` [([link](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html)) including: The profiles expected to be used for the resources resolved to by the ... `draftOrders` context element [are] [profile-devicerequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-devicerequest.html), [profile-medicationrequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-medicationrequest.html), [profile-nutritionorder](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-nutritionorder.html), [profile-visionprescription](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-visionprescription.html),  [profile-servicerequest](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-servicerequest.html)]</t>
+  </si>
+  <si>
+    <t>Use and profiles for [order-select](https://hl7.org/fhir/us/davinci-crd/STU2/hooks.html#order-select) also apply to `order-sign` [([link](https://cds-hooks.hl7.org/hooks/STU1/order-sign.html)) including: while this hook does not explicitly list PractitionerRole [([us-core-practitionerrole](http://hl7.org/fhir/us/core/STU3.1.1/StructureDefinition-us-core-practitionerrole.html)) in addition to  [profile-practitioner](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-practitioner.html)] as an expected resource type for userId, it is not prohibited and is included to allow linking the user to a Practitioner in a specific role acting on behalf of a specific Organization.]</t>
+  </si>
+  <si>
+    <t>[In response to an [encounter-discharge](https://cds-hooks.hl7.org/hooks/encounter-discharge/STU1/encounter-discharge/) hook call, [clients should v]erify that documentation requirements for the services performed have been met to ensure the services provided can be reimbursed</t>
+  </si>
+  <si>
+    <t>[In response to an [encounter-discharge](https://cds-hooks.hl7.org/hooks/encounter-discharge/STU1/encounter-discharge/) hook call, [clients should e]nsure that required follow-up planning is complete and appropriate transfer of care has been arranged, particularly for accountable care models</t>
+  </si>
+  <si>
+    <t>FHIR API</t>
+  </si>
+  <si>
+    <t>User Interaction</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Prefetch</t>
+  </si>
+  <si>
+    <t>What if</t>
+  </si>
+  <si>
+    <t>CRD Request</t>
+  </si>
+  <si>
+    <t>Logging</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>CRD Configuration</t>
+  </si>
+  <si>
+    <t>Resource creation</t>
+  </si>
+  <si>
+    <t>User interaction</t>
+  </si>
+  <si>
+    <t>Deprecated because this is a detail that implementers need to be aware of and handle based on internal implementation choices, but that an external system performing verification won't see or need to check explicitly. 72 is the real requirement.</t>
+  </si>
+  <si>
+    <t>Hook - appointment-book</t>
+  </si>
+  <si>
+    <t>Hook - encounter-start</t>
+  </si>
+  <si>
+    <t>Card - External reference</t>
+  </si>
+  <si>
+    <t>Card - Coverage information</t>
+  </si>
+  <si>
+    <t>Hook - encounter-discharge</t>
+  </si>
+  <si>
+    <t>Card - Identify additional orders</t>
+  </si>
+  <si>
+    <t>Card - Instructions</t>
+  </si>
+  <si>
+    <t>Hook - order-dispatch</t>
+  </si>
+  <si>
+    <t>Hook - order-select</t>
+  </si>
+  <si>
+    <t>Hook - order-sign</t>
+  </si>
+  <si>
+    <t>Card - Propose alternate request</t>
+  </si>
+  <si>
+    <t>Card - Create or update coverage information</t>
+  </si>
+  <si>
+    <t>Card - Request form completion</t>
   </si>
 </sst>
 </file>
@@ -3453,6 +3531,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3471,20 +3563,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3853,14 +3931,14 @@
       <c r="C3" s="14"/>
     </row>
     <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
-        <v>442</v>
+      <c r="A4" s="43" t="s">
+        <v>421</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="19"/>
       <c r="C5" s="14"/>
     </row>
@@ -3872,17 +3950,17 @@
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="46"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="39"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="47"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="35"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="18"/>
     </row>
     <row r="10" spans="1:3" ht="292" x14ac:dyDescent="0.2">
@@ -3908,10 +3986,10 @@
   <dimension ref="A1:AE434"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A219" sqref="A219:A226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3939,68 +4017,68 @@
     <col min="22" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="47" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:31" s="41" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="41" t="s">
-        <v>443</v>
-      </c>
-      <c r="F1" s="42" t="s">
+      <c r="E1" s="35" t="s">
+        <v>422</v>
+      </c>
+      <c r="F1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="I1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="S1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="43" t="s">
+      <c r="T1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="48"/>
+      <c r="Y1" s="42"/>
     </row>
     <row r="2" spans="1:31" s="24" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="25">
@@ -4063,6 +4141,9 @@
       <c r="N3" s="30" t="s">
         <v>35</v>
       </c>
+      <c r="P3" s="27" t="s">
+        <v>451</v>
+      </c>
       <c r="T3" s="27" t="s">
         <v>36</v>
       </c>
@@ -4361,10 +4442,10 @@
         <v>41</v>
       </c>
       <c r="T16" s="27" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="25">
         <v>16</v>
       </c>
@@ -4384,7 +4465,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="25">
         <v>17</v>
       </c>
@@ -4408,7 +4489,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="25">
         <v>18</v>
       </c>
@@ -4428,7 +4509,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="25">
         <v>19</v>
       </c>
@@ -4448,7 +4529,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A21" s="25">
         <v>20</v>
       </c>
@@ -4472,7 +4553,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="25">
         <v>21</v>
       </c>
@@ -4487,6 +4568,12 @@
       </c>
       <c r="E22" s="25" t="s">
         <v>34</v>
+      </c>
+      <c r="G22" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>429</v>
       </c>
       <c r="M22" s="30" t="str" cm="1">
         <f t="array" ref="M22">PAGE_NAME(B22)</f>
@@ -4495,8 +4582,11 @@
       <c r="N22" s="30" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="P22" s="27" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="25">
         <v>22</v>
       </c>
@@ -4516,7 +4606,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A24" s="25">
         <v>23</v>
       </c>
@@ -4540,7 +4630,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A25" s="25">
         <v>24</v>
       </c>
@@ -4564,7 +4654,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A26" s="25">
         <v>25</v>
       </c>
@@ -4588,7 +4678,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="25">
         <v>26</v>
       </c>
@@ -4612,7 +4702,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="25">
         <v>27</v>
       </c>
@@ -4636,7 +4726,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A29" s="25">
         <v>28</v>
       </c>
@@ -4660,7 +4750,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="25">
         <v>29</v>
       </c>
@@ -4684,7 +4774,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A31" s="25">
         <v>30</v>
       </c>
@@ -4707,8 +4797,11 @@
       <c r="N31" s="30" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P31" s="27" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="25">
         <v>31</v>
       </c>
@@ -4731,8 +4824,11 @@
       <c r="N32" s="30" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P32" s="27" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="25">
         <v>32</v>
       </c>
@@ -4755,8 +4851,11 @@
       <c r="N33" s="30" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P33" s="27" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="25">
         <v>33</v>
       </c>
@@ -4779,8 +4878,11 @@
       <c r="N34" s="30" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="P34" s="27" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" s="25">
         <v>34</v>
       </c>
@@ -4800,7 +4902,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A36" s="25">
         <v>35</v>
       </c>
@@ -4820,7 +4922,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A37" s="25">
         <v>36</v>
       </c>
@@ -4840,7 +4942,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="25">
         <v>37</v>
       </c>
@@ -4860,7 +4962,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" s="25">
         <v>38</v>
       </c>
@@ -4880,7 +4982,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="25">
         <v>39</v>
       </c>
@@ -4888,7 +4990,7 @@
         <v>87</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
       <c r="D40" s="25" t="s">
         <v>50</v>
@@ -4904,7 +5006,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="25">
         <v>40</v>
       </c>
@@ -4928,7 +5030,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" s="25">
         <v>41</v>
       </c>
@@ -4952,7 +5054,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="25">
         <v>42</v>
       </c>
@@ -4972,7 +5074,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="221" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="221" x14ac:dyDescent="0.2">
       <c r="A44" s="25">
         <v>43</v>
       </c>
@@ -4995,8 +5097,11 @@
       <c r="N44" s="30" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+      <c r="P44" s="27" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A45" s="25">
         <v>44</v>
       </c>
@@ -5020,7 +5125,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="170" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="170" x14ac:dyDescent="0.2">
       <c r="A46" s="25">
         <v>45</v>
       </c>
@@ -5044,7 +5149,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="25">
         <v>46</v>
       </c>
@@ -5068,7 +5173,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="187" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="187" x14ac:dyDescent="0.2">
       <c r="A48" s="25">
         <v>47</v>
       </c>
@@ -5259,6 +5364,9 @@
       <c r="N55" s="30" t="s">
         <v>95</v>
       </c>
+      <c r="P55" s="27" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="56" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="25">
@@ -5308,7 +5416,7 @@
         <v>110</v>
       </c>
       <c r="T57" s="27" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="119" x14ac:dyDescent="0.2">
@@ -5475,7 +5583,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" s="25">
         <v>64</v>
       </c>
@@ -5494,8 +5602,11 @@
       <c r="N65" s="30" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P65" s="27" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A66" s="25">
         <v>65</v>
       </c>
@@ -5514,8 +5625,11 @@
       <c r="N66" s="30" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="P66" s="27" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A67" s="25">
         <v>66</v>
       </c>
@@ -5534,8 +5648,11 @@
       <c r="N67" s="30" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P67" s="27" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A68" s="25">
         <v>67</v>
       </c>
@@ -5559,7 +5676,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="25">
         <v>68</v>
       </c>
@@ -5583,7 +5700,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="25">
         <v>69</v>
       </c>
@@ -5602,8 +5719,11 @@
       <c r="N70" s="30" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="P70" s="27" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="25">
         <v>70</v>
       </c>
@@ -5623,7 +5743,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="25">
         <v>71</v>
       </c>
@@ -5646,8 +5766,11 @@
       <c r="N72" s="30" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P72" s="27" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A73" s="25">
         <v>72</v>
       </c>
@@ -5666,8 +5789,11 @@
       <c r="N73" s="30" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="P73" s="27" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A74" s="25">
         <v>73</v>
       </c>
@@ -5678,7 +5804,7 @@
         <v>134</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>33</v>
+        <v>206</v>
       </c>
       <c r="E74" s="25" t="s">
         <v>34</v>
@@ -5690,8 +5816,14 @@
       <c r="N74" s="30" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P74" s="27" t="s">
+        <v>456</v>
+      </c>
+      <c r="T74" s="27" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A75" s="25">
         <v>74</v>
       </c>
@@ -5702,13 +5834,19 @@
         <v>135</v>
       </c>
       <c r="D75" s="25" t="s">
-        <v>33</v>
+        <v>206</v>
       </c>
       <c r="E75" s="25" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="P75" s="27" t="s">
+        <v>456</v>
+      </c>
+      <c r="T75" s="27" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A76" s="25">
         <v>75</v>
       </c>
@@ -5731,8 +5869,11 @@
       <c r="N76" s="30" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="P76" s="27" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A77" s="25">
         <v>76</v>
       </c>
@@ -5756,7 +5897,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="25">
         <v>77</v>
       </c>
@@ -5776,7 +5917,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A79" s="25">
         <v>78</v>
       </c>
@@ -5795,8 +5936,11 @@
       <c r="N79" s="30" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="P79" s="27" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="25">
         <v>79</v>
       </c>
@@ -5819,6 +5963,9 @@
       <c r="N80" s="30" t="s">
         <v>132</v>
       </c>
+      <c r="P80" s="27" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="81" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="25">
@@ -5843,6 +5990,9 @@
       <c r="N81" s="30" t="s">
         <v>132</v>
       </c>
+      <c r="P81" s="27" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="82" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="25">
@@ -5916,6 +6066,9 @@
         <f t="array" ref="N84">SECTION_NAME(B84)</f>
         <v>privacy-security-and-safety</v>
       </c>
+      <c r="P84" s="27" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="85" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A85" s="25">
@@ -5933,6 +6086,9 @@
       <c r="E85" s="25" t="s">
         <v>29</v>
       </c>
+      <c r="P85" s="27" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="86" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A86" s="25">
@@ -5950,6 +6106,9 @@
       <c r="E86" s="25" t="s">
         <v>29</v>
       </c>
+      <c r="P86" s="27" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="87" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A87" s="25">
@@ -5975,8 +6134,11 @@
         <f t="array" ref="N87">SECTION_NAME(B87)</f>
         <v>privacy-security-and-safety</v>
       </c>
+      <c r="P87" s="27" t="s">
+        <v>458</v>
+      </c>
       <c r="T87" s="27" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
     </row>
     <row r="88" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -6003,6 +6165,9 @@
         <f t="array" ref="N88">SECTION_NAME(B88)</f>
         <v>privacy-security-and-safety</v>
       </c>
+      <c r="P88" s="27" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="89" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A89" s="25">
@@ -6028,6 +6193,9 @@
         <f t="array" ref="N89">SECTION_NAME(B89)</f>
         <v>privacy-security-and-safety</v>
       </c>
+      <c r="P89" s="27" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="90" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="25">
@@ -6053,6 +6221,9 @@
         <f t="array" ref="N90">SECTION_NAME(B90)</f>
         <v>privacy-security-and-safety</v>
       </c>
+      <c r="P90" s="27" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="91" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="25">
@@ -6104,7 +6275,7 @@
         <v>privacy-security-and-safety</v>
       </c>
       <c r="T92" s="27" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
     </row>
     <row r="93" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -6131,6 +6302,9 @@
         <f t="array" ref="N93">SECTION_NAME(B93)</f>
         <v>privacy-security-and-safety</v>
       </c>
+      <c r="P93" s="27" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="94" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="25">
@@ -6273,6 +6447,9 @@
         <f t="array" ref="N99">SECTION_NAME(B99)</f>
         <v>privacy-security-and-safety</v>
       </c>
+      <c r="P99" s="27" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="100" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A100" s="25">
@@ -6323,8 +6500,11 @@
         <f t="array" ref="N101">SECTION_NAME(B101)</f>
         <v>privacy-security-and-safety</v>
       </c>
+      <c r="P101" s="27" t="s">
+        <v>458</v>
+      </c>
       <c r="T101" s="27" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
     </row>
     <row r="102" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -6602,7 +6782,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A113" s="25">
         <v>112</v>
       </c>
@@ -6627,7 +6807,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A114" s="25">
         <v>113</v>
       </c>
@@ -6652,7 +6832,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A115" s="25">
         <v>114</v>
       </c>
@@ -6677,7 +6857,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A116" s="25">
         <v>115</v>
       </c>
@@ -6702,7 +6882,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A117" s="25">
         <v>116</v>
       </c>
@@ -6727,7 +6907,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A118" s="25">
         <v>117</v>
       </c>
@@ -6752,7 +6932,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A119" s="25">
         <v>118</v>
       </c>
@@ -6777,7 +6957,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A120" s="25">
         <v>119</v>
       </c>
@@ -6802,7 +6982,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="25">
         <v>120</v>
       </c>
@@ -6827,7 +7007,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A122" s="25">
         <v>121</v>
       </c>
@@ -6852,7 +7032,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A123" s="25">
         <v>122</v>
       </c>
@@ -6877,7 +7057,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A124" s="25">
         <v>123</v>
       </c>
@@ -6902,7 +7082,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A125" s="25">
         <v>124</v>
       </c>
@@ -6927,7 +7107,7 @@
         <v>configuration-options-extension</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A126" s="25">
         <v>125</v>
       </c>
@@ -6952,7 +7132,7 @@
         <v>hook-configuration-extension</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A127" s="25">
         <v>126</v>
       </c>
@@ -6976,8 +7156,11 @@
         <f t="array" ref="N127">SECTION_NAME(B127)</f>
         <v>hook-configuration-extension</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="P127" s="27" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A128" s="25">
         <v>127</v>
       </c>
@@ -7126,8 +7309,11 @@
         <f t="array" ref="N133">SECTION_NAME(B133)</f>
         <v>additional-prefetch-capabilities</v>
       </c>
+      <c r="P133" s="27" t="s">
+        <v>454</v>
+      </c>
       <c r="T133" s="27" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
     </row>
     <row r="134" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -7154,6 +7340,9 @@
         <f t="array" ref="N134">SECTION_NAME(B134)</f>
         <v>additional-prefetch-capabilities</v>
       </c>
+      <c r="P134" s="27" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="135" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A135" s="25">
@@ -7180,7 +7369,7 @@
         <v>additional-response-capabilities</v>
       </c>
       <c r="T135" s="27" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
     </row>
     <row r="136" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -7249,6 +7438,9 @@
         <f t="array" ref="N138">SECTION_NAME(B138)</f>
         <v>linkage-between-created-resources</v>
       </c>
+      <c r="P138" s="27" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="139" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A139" s="25">
@@ -7274,6 +7466,9 @@
         <f t="array" ref="N139">SECTION_NAME(B139)</f>
         <v>linkage-between-created-resources</v>
       </c>
+      <c r="P139" s="27" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="140" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A140" s="25">
@@ -7299,6 +7494,9 @@
         <f t="array" ref="N140">SECTION_NAME(B140)</f>
         <v>linkage-between-created-resources</v>
       </c>
+      <c r="P140" s="27" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="141" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A141" s="25">
@@ -7374,6 +7572,9 @@
         <f t="array" ref="N143">SECTION_NAME(B143)</f>
         <v>controlling-hook-invocation</v>
       </c>
+      <c r="P143" s="27" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="144" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A144" s="25">
@@ -7424,6 +7625,9 @@
         <f t="array" ref="N145">SECTION_NAME(B145)</f>
         <v>controlling-hook-invocation</v>
       </c>
+      <c r="P145" s="27" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="146" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A146" s="25">
@@ -7449,6 +7653,9 @@
         <f t="array" ref="N146">SECTION_NAME(B146)</f>
         <v>controlling-hook-invocation</v>
       </c>
+      <c r="P146" s="27" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="147" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A147" s="25">
@@ -7474,6 +7681,9 @@
         <f t="array" ref="N147">SECTION_NAME(B147)</f>
         <v>controlling-hook-invocation</v>
       </c>
+      <c r="P147" s="27" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="148" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="25">
@@ -7524,6 +7734,9 @@
         <f t="array" ref="N149">SECTION_NAME(B149)</f>
         <v>supported-hooks</v>
       </c>
+      <c r="P149" s="27" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="150" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A150" s="25">
@@ -7549,6 +7762,9 @@
         <f t="array" ref="N150">SECTION_NAME(B150)</f>
         <v>supported-hooks</v>
       </c>
+      <c r="P150" s="27" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="151" spans="1:20" ht="407" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="25">
@@ -7574,6 +7790,9 @@
         <f t="array" ref="N151">SECTION_NAME(B151)</f>
         <v>supported-hooks</v>
       </c>
+      <c r="P151" s="27" t="s">
+        <v>456</v>
+      </c>
       <c r="T151" s="27" t="s">
         <v>228</v>
       </c>
@@ -7803,7 +8022,7 @@
         <v>supported-hooks</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A161" s="25">
         <v>160</v>
       </c>
@@ -7828,7 +8047,7 @@
         <v>supported-hooks</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A162" s="25">
         <v>161</v>
       </c>
@@ -7853,7 +8072,7 @@
         <v>supported-hooks</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A163" s="25">
         <v>162</v>
       </c>
@@ -7878,7 +8097,7 @@
         <v>supported-hooks</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A164" s="25">
         <v>163</v>
       </c>
@@ -7903,7 +8122,7 @@
         <v>supported-hooks</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="221" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" ht="221" x14ac:dyDescent="0.2">
       <c r="A165" s="25">
         <v>164</v>
       </c>
@@ -7924,7 +8143,7 @@
         <v>hook-categories</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A166" s="25">
         <v>165</v>
       </c>
@@ -7945,7 +8164,7 @@
         <v>hook-categories</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A167" s="25">
         <v>166</v>
       </c>
@@ -7966,7 +8185,7 @@
         <v>hook-categories</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="255" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" ht="255" x14ac:dyDescent="0.2">
       <c r="A168" s="25">
         <v>167</v>
       </c>
@@ -7974,7 +8193,7 @@
         <v>242</v>
       </c>
       <c r="C168" s="25" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="D168" s="25" t="s">
         <v>157</v>
@@ -7987,7 +8206,7 @@
         <v>hook-categories</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A169" s="25">
         <v>168</v>
       </c>
@@ -8008,7 +8227,7 @@
         <v>hook-categories</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A170" s="25">
         <v>169</v>
       </c>
@@ -8033,7 +8252,7 @@
         <v>appointment-book</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A171" s="25">
         <v>170</v>
       </c>
@@ -8054,7 +8273,7 @@
         <v>appointment-book</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A172" s="25">
         <v>171</v>
       </c>
@@ -8074,8 +8293,11 @@
         <f t="array" ref="N172">SECTION_NAME(B173)</f>
         <v>appointment-book</v>
       </c>
-    </row>
-    <row r="173" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="P172" s="27" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A173" s="25">
         <v>172</v>
       </c>
@@ -8095,8 +8317,11 @@
         <f t="array" ref="N173">SECTION_NAME(B174)</f>
         <v>appointment-book</v>
       </c>
-    </row>
-    <row r="174" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="P173" s="27" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A174" s="25">
         <v>173</v>
       </c>
@@ -8117,7 +8342,7 @@
         <v>appointment-book</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A175" s="25">
         <v>174</v>
       </c>
@@ -8138,7 +8363,7 @@
         <v>appointment-book</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A176" s="25">
         <v>175</v>
       </c>
@@ -8191,7 +8416,7 @@
         <v>256</v>
       </c>
       <c r="D178" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E178" s="25" t="s">
         <v>34</v>
@@ -8200,6 +8425,9 @@
         <f t="array" ref="N178">SECTION_NAME(B179)</f>
         <v>appointment-book</v>
       </c>
+      <c r="P178" s="27" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="179" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A179" s="25">
@@ -8212,7 +8440,7 @@
         <v>257</v>
       </c>
       <c r="D179" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E179" s="25" t="s">
         <v>34</v>
@@ -8221,6 +8449,9 @@
         <f t="array" ref="N179">SECTION_NAME(B180)</f>
         <v>appointment-book</v>
       </c>
+      <c r="P179" s="27" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="180" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A180" s="25">
@@ -8233,7 +8464,7 @@
         <v>258</v>
       </c>
       <c r="D180" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E180" s="25" t="s">
         <v>34</v>
@@ -8242,6 +8473,9 @@
         <f t="array" ref="N180">SECTION_NAME(B181)</f>
         <v>appointment-book</v>
       </c>
+      <c r="P180" s="27" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="181" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A181" s="25">
@@ -8254,7 +8488,7 @@
         <v>259</v>
       </c>
       <c r="D181" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E181" s="25" t="s">
         <v>34</v>
@@ -8263,6 +8497,9 @@
         <f t="array" ref="N181">SECTION_NAME(B182)</f>
         <v>appointment-book</v>
       </c>
+      <c r="P181" s="27" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="182" spans="1:21" ht="153" x14ac:dyDescent="0.2">
       <c r="A182" s="25">
@@ -8338,6 +8575,9 @@
         <f t="array" ref="N184">SECTION_NAME(B184)</f>
         <v>appointment-book</v>
       </c>
+      <c r="P184" s="27" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="185" spans="1:21" ht="102" x14ac:dyDescent="0.2">
       <c r="A185" s="25">
@@ -8406,6 +8646,9 @@
         <f t="array" ref="N187">SECTION_NAME(B187)</f>
         <v>encounter-start</v>
       </c>
+      <c r="P187" s="27" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="188" spans="1:21" ht="85" x14ac:dyDescent="0.2">
       <c r="A188" s="25">
@@ -8427,6 +8670,9 @@
         <f t="array" ref="N188">SECTION_NAME(B188)</f>
         <v>encounter-start</v>
       </c>
+      <c r="P188" s="27" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="189" spans="1:21" ht="187" x14ac:dyDescent="0.2">
       <c r="A189" s="25">
@@ -8449,7 +8695,7 @@
         <v>encounter-start</v>
       </c>
       <c r="T189" s="27" t="s">
-        <v>448</v>
+        <v>427</v>
       </c>
     </row>
     <row r="190" spans="1:21" ht="136" x14ac:dyDescent="0.2">
@@ -8526,7 +8772,7 @@
         <v>272</v>
       </c>
       <c r="D193" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E193" s="25" t="s">
         <v>34</v>
@@ -8535,6 +8781,9 @@
         <f t="array" ref="N193">SECTION_NAME(B193)</f>
         <v>encounter-start</v>
       </c>
+      <c r="P193" s="27" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="194" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A194" s="25">
@@ -8547,7 +8796,7 @@
         <v>273</v>
       </c>
       <c r="D194" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E194" s="25" t="s">
         <v>34</v>
@@ -8556,6 +8805,9 @@
         <f t="array" ref="N194">SECTION_NAME(B194)</f>
         <v>encounter-start</v>
       </c>
+      <c r="P194" s="27" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="195" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A195" s="25">
@@ -8568,7 +8820,7 @@
         <v>274</v>
       </c>
       <c r="D195" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E195" s="25" t="s">
         <v>34</v>
@@ -8581,6 +8833,9 @@
         <f t="array" ref="N195">SECTION_NAME(B195)</f>
         <v>encounter-start</v>
       </c>
+      <c r="P195" s="27" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="196" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A196" s="25">
@@ -8640,6 +8895,9 @@
       <c r="E198" s="25" t="s">
         <v>34</v>
       </c>
+      <c r="P198" s="27" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="199" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A199" s="25">
@@ -8666,7 +8924,7 @@
         <v>276</v>
       </c>
       <c r="C200" s="25" t="s">
-        <v>280</v>
+        <v>449</v>
       </c>
       <c r="D200" s="25" t="s">
         <v>50</v>
@@ -8683,7 +8941,7 @@
         <v>276</v>
       </c>
       <c r="C201" s="25" t="s">
-        <v>281</v>
+        <v>450</v>
       </c>
       <c r="D201" s="25" t="s">
         <v>50</v>
@@ -8700,13 +8958,16 @@
         <v>276</v>
       </c>
       <c r="C202" s="25" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D202" s="25" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E202" s="25" t="s">
         <v>34</v>
+      </c>
+      <c r="P202" s="27" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="203" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -8717,13 +8978,16 @@
         <v>276</v>
       </c>
       <c r="C203" s="25" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D203" s="25" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E203" s="25" t="s">
         <v>34</v>
+      </c>
+      <c r="P203" s="27" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="204" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -8734,10 +8998,10 @@
         <v>276</v>
       </c>
       <c r="C204" s="25" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D204" s="25" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E204" s="25" t="s">
         <v>34</v>
@@ -8750,25 +9014,28 @@
         <f t="array" ref="N204">SECTION_NAME(B204)</f>
         <v>encounter-discharge</v>
       </c>
+      <c r="P204" s="27" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="205" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A205" s="25">
         <v>204</v>
       </c>
       <c r="B205" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="C205" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="D205" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E205" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="T205" s="27" t="s">
         <v>285</v>
-      </c>
-      <c r="C205" s="25" t="s">
-        <v>286</v>
-      </c>
-      <c r="D205" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E205" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="T205" s="27" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="206" spans="1:20" ht="85" x14ac:dyDescent="0.2">
@@ -8776,19 +9043,22 @@
         <v>205</v>
       </c>
       <c r="B206" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="C206" s="25" t="s">
+        <v>286</v>
+      </c>
+      <c r="D206" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E206" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="P206" s="27" t="s">
+        <v>470</v>
+      </c>
+      <c r="T206" s="27" t="s">
         <v>285</v>
-      </c>
-      <c r="C206" s="25" t="s">
-        <v>288</v>
-      </c>
-      <c r="D206" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E206" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="T206" s="27" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="207" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -8796,10 +9066,10 @@
         <v>206</v>
       </c>
       <c r="B207" s="33" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C207" s="25" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D207" s="25" t="s">
         <v>28</v>
@@ -8816,7 +9086,7 @@
         <v>order-dispatch</v>
       </c>
       <c r="T207" s="27" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="208" spans="1:20" ht="119" x14ac:dyDescent="0.2">
@@ -8824,10 +9094,10 @@
         <v>207</v>
       </c>
       <c r="B208" s="33" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C208" s="25" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D208" s="25" t="s">
         <v>33</v>
@@ -8843,19 +9113,22 @@
         <f t="array" ref="N208">SECTION_NAME(B208)</f>
         <v>order-dispatch</v>
       </c>
+      <c r="P208" s="27" t="s">
+        <v>470</v>
+      </c>
       <c r="T208" s="27" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="209" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="209" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A209" s="25">
         <v>208</v>
       </c>
       <c r="B209" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C209" s="25" t="s">
-        <v>292</v>
+        <v>432</v>
       </c>
       <c r="D209" s="25" t="s">
         <v>33</v>
@@ -8864,18 +9137,18 @@
         <v>38</v>
       </c>
       <c r="T209" s="27" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="210" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="210" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A210" s="25">
         <v>209</v>
       </c>
       <c r="B210" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C210" s="25" t="s">
-        <v>294</v>
+        <v>433</v>
       </c>
       <c r="D210" s="25" t="s">
         <v>33</v>
@@ -8883,8 +9156,11 @@
       <c r="E210" s="25" t="s">
         <v>34</v>
       </c>
+      <c r="P210" s="27" t="s">
+        <v>471</v>
+      </c>
       <c r="T210" s="27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="211" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -8892,10 +9168,10 @@
         <v>210</v>
       </c>
       <c r="B211" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C211" s="25" t="s">
-        <v>295</v>
+        <v>434</v>
       </c>
       <c r="D211" s="25" t="s">
         <v>50</v>
@@ -8917,10 +9193,10 @@
         <v>211</v>
       </c>
       <c r="B212" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C212" s="25" t="s">
-        <v>296</v>
+        <v>435</v>
       </c>
       <c r="D212" s="25" t="s">
         <v>50</v>
@@ -8942,16 +9218,19 @@
         <v>212</v>
       </c>
       <c r="B213" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C213" s="25" t="s">
-        <v>297</v>
+        <v>436</v>
       </c>
       <c r="D213" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E213" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="P213" s="27" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="214" spans="1:20" ht="85" x14ac:dyDescent="0.2">
@@ -8959,33 +9238,36 @@
         <v>213</v>
       </c>
       <c r="B214" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C214" s="25" t="s">
-        <v>298</v>
+        <v>437</v>
       </c>
       <c r="D214" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E214" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="215" spans="1:20" ht="255" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="P214" s="27" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="215" spans="1:20" ht="238" x14ac:dyDescent="0.2">
       <c r="A215" s="25">
         <v>214</v>
       </c>
       <c r="B215" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C215" s="25" t="s">
-        <v>299</v>
+        <v>438</v>
       </c>
       <c r="D215" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E215" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M215" s="30" t="str" cm="1">
         <f t="array" ref="M215">PAGE_NAME(B215)</f>
@@ -8995,22 +9277,28 @@
         <f t="array" ref="N215">SECTION_NAME(B215)</f>
         <v>order-select</v>
       </c>
+      <c r="P215" s="27" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="216" spans="1:20" ht="170" x14ac:dyDescent="0.2">
       <c r="A216" s="25">
         <v>215</v>
       </c>
       <c r="B216" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C216" s="25" t="s">
-        <v>300</v>
+        <v>439</v>
       </c>
       <c r="D216" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E216" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="P216" s="27" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="217" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -9018,16 +9306,16 @@
         <v>216</v>
       </c>
       <c r="B217" s="33" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C217" s="25" t="s">
-        <v>301</v>
+        <v>440</v>
       </c>
       <c r="D217" s="25" t="s">
         <v>28</v>
       </c>
       <c r="E217" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M217" s="30" t="str" cm="1">
         <f t="array" ref="M217">PAGE_NAME(B217)</f>
@@ -9043,10 +9331,10 @@
         <v>217</v>
       </c>
       <c r="B218" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C218" s="25" t="s">
-        <v>303</v>
+        <v>431</v>
       </c>
       <c r="D218" s="25" t="s">
         <v>33</v>
@@ -9060,16 +9348,19 @@
         <v>218</v>
       </c>
       <c r="B219" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C219" s="25" t="s">
-        <v>304</v>
+        <v>430</v>
       </c>
       <c r="D219" s="25" t="s">
         <v>33</v>
       </c>
       <c r="E219" s="25" t="s">
         <v>34</v>
+      </c>
+      <c r="P219" s="27" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="220" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -9077,10 +9368,10 @@
         <v>219</v>
       </c>
       <c r="B220" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C220" s="25" t="s">
-        <v>305</v>
+        <v>441</v>
       </c>
       <c r="D220" s="25" t="s">
         <v>28</v>
@@ -9102,16 +9393,19 @@
         <v>220</v>
       </c>
       <c r="B221" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C221" s="25" t="s">
-        <v>306</v>
+        <v>445</v>
       </c>
       <c r="D221" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E221" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="P221" s="27" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="222" spans="1:20" ht="136" x14ac:dyDescent="0.2">
@@ -9119,16 +9413,16 @@
         <v>221</v>
       </c>
       <c r="B222" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C222" s="25" t="s">
-        <v>307</v>
+        <v>446</v>
       </c>
       <c r="D222" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E222" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M222" s="30" t="str" cm="1">
         <f t="array" ref="M222">PAGE_NAME(B222)</f>
@@ -9138,22 +9432,28 @@
         <f t="array" ref="N222">SECTION_NAME(B222)</f>
         <v>order-sign</v>
       </c>
+      <c r="P222" s="27" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="223" spans="1:20" ht="289" x14ac:dyDescent="0.2">
       <c r="A223" s="25">
         <v>222</v>
       </c>
       <c r="B223" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C223" s="25" t="s">
-        <v>308</v>
+        <v>447</v>
       </c>
       <c r="D223" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E223" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="P223" s="27" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="224" spans="1:20" ht="221" x14ac:dyDescent="0.2">
@@ -9161,27 +9461,30 @@
         <v>223</v>
       </c>
       <c r="B224" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C224" s="25" t="s">
-        <v>309</v>
+        <v>448</v>
       </c>
       <c r="D224" s="25" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E224" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="225" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="P224" s="27" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A225" s="25">
         <v>224</v>
       </c>
       <c r="B225" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C225" s="25" t="s">
-        <v>310</v>
+        <v>442</v>
       </c>
       <c r="D225" s="25" t="s">
         <v>28</v>
@@ -9198,15 +9501,15 @@
         <v>order-sign</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A226" s="25">
         <v>225</v>
       </c>
       <c r="B226" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C226" s="25" t="s">
-        <v>311</v>
+        <v>443</v>
       </c>
       <c r="D226" s="25" t="s">
         <v>33</v>
@@ -9222,16 +9525,19 @@
         <f t="array" ref="N226">SECTION_NAME(B226)</f>
         <v>order-sign</v>
       </c>
-    </row>
-    <row r="227" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P226" s="27" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A227" s="25">
         <v>226</v>
       </c>
       <c r="B227" s="33" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C227" s="25" t="s">
-        <v>312</v>
+        <v>444</v>
       </c>
       <c r="D227" s="25" t="s">
         <v>33</v>
@@ -9248,15 +9554,15 @@
         <v>order-sign</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A228" s="25">
         <v>227</v>
       </c>
       <c r="B228" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C228" s="25" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="D228" s="25" t="s">
         <v>50</v>
@@ -9273,15 +9579,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A229" s="25">
         <v>228</v>
       </c>
       <c r="B229" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C229" s="25" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
       <c r="D229" s="25" t="s">
         <v>50</v>
@@ -9298,15 +9604,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A230" s="25">
         <v>229</v>
       </c>
       <c r="B230" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C230" s="25" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="D230" s="25" t="s">
         <v>50</v>
@@ -9323,15 +9629,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A231" s="25">
         <v>230</v>
       </c>
       <c r="B231" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C231" s="25" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
       <c r="D231" s="25" t="s">
         <v>50</v>
@@ -9348,15 +9654,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A232" s="25">
         <v>231</v>
       </c>
       <c r="B232" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C232" s="25" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="D232" s="25" t="s">
         <v>50</v>
@@ -9373,15 +9679,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A233" s="25">
         <v>232</v>
       </c>
       <c r="B233" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C233" s="25" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="D233" s="25" t="s">
         <v>50</v>
@@ -9398,15 +9704,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A234" s="25">
         <v>233</v>
       </c>
       <c r="B234" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C234" s="25" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
       <c r="D234" s="25" t="s">
         <v>50</v>
@@ -9423,15 +9729,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A235" s="25">
         <v>234</v>
       </c>
       <c r="B235" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C235" s="25" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="D235" s="25" t="s">
         <v>50</v>
@@ -9448,15 +9754,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A236" s="25">
         <v>235</v>
       </c>
       <c r="B236" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C236" s="25" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="D236" s="25" t="s">
         <v>50</v>
@@ -9473,15 +9779,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A237" s="25">
         <v>236</v>
       </c>
       <c r="B237" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C237" s="25" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="D237" s="25" t="s">
         <v>50</v>
@@ -9498,15 +9804,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A238" s="25">
         <v>237</v>
       </c>
       <c r="B238" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C238" s="25" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
       <c r="D238" s="25" t="s">
         <v>50</v>
@@ -9523,15 +9829,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A239" s="25">
         <v>238</v>
       </c>
       <c r="B239" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C239" s="25" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="D239" s="25" t="s">
         <v>50</v>
@@ -9548,15 +9854,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A240" s="25">
         <v>239</v>
       </c>
       <c r="B240" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C240" s="25" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="D240" s="25" t="s">
         <v>50</v>
@@ -9573,15 +9879,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A241" s="25">
         <v>240</v>
       </c>
       <c r="B241" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C241" s="25" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="D241" s="25" t="s">
         <v>50</v>
@@ -9598,15 +9904,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A242" s="25">
         <v>241</v>
       </c>
       <c r="B242" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C242" s="25" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="D242" s="25" t="s">
         <v>105</v>
@@ -9623,15 +9929,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A243" s="25">
         <v>242</v>
       </c>
       <c r="B243" s="33" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C243" s="25" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="D243" s="25" t="s">
         <v>50</v>
@@ -9648,15 +9954,15 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A244" s="25">
         <v>243</v>
       </c>
       <c r="B244" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C244" s="25" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="D244" s="25" t="s">
         <v>33</v>
@@ -9672,16 +9978,19 @@
         <f t="array" ref="N244">SECTION_NAME(B244)</f>
         <v>potential-crd-response-types</v>
       </c>
-    </row>
-    <row r="245" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="P244" s="27" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="245" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A245" s="25">
         <v>244</v>
       </c>
       <c r="B245" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C245" s="25" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="D245" s="25" t="s">
         <v>33</v>
@@ -9697,16 +10006,19 @@
         <f t="array" ref="N245">SECTION_NAME(B245)</f>
         <v>potential-crd-response-types</v>
       </c>
-    </row>
-    <row r="246" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="P245" s="27" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="246" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A246" s="25">
         <v>245</v>
       </c>
       <c r="B246" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C246" s="25" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="D246" s="25" t="s">
         <v>33</v>
@@ -9722,16 +10034,19 @@
         <f t="array" ref="N246">SECTION_NAME(B246)</f>
         <v>potential-crd-response-types</v>
       </c>
-    </row>
-    <row r="247" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="P246" s="27" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="247" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A247" s="25">
         <v>246</v>
       </c>
       <c r="B247" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C247" s="25" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="D247" s="25" t="s">
         <v>50</v>
@@ -9748,15 +10063,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="248" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A248" s="25">
         <v>247</v>
       </c>
       <c r="B248" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C248" s="25" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="D248" s="25" t="s">
         <v>33</v>
@@ -9773,15 +10088,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A249" s="25">
         <v>248</v>
       </c>
       <c r="B249" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C249" s="25" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
       <c r="D249" s="25" t="s">
         <v>33</v>
@@ -9798,15 +10113,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A250" s="25">
         <v>249</v>
       </c>
       <c r="B250" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C250" s="25" t="s">
-        <v>337</v>
+        <v>316</v>
       </c>
       <c r="D250" s="25" t="s">
         <v>33</v>
@@ -9823,15 +10138,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A251" s="25">
         <v>250</v>
       </c>
       <c r="B251" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C251" s="25" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="D251" s="25" t="s">
         <v>28</v>
@@ -9848,15 +10163,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="252" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A252" s="25">
         <v>251</v>
       </c>
       <c r="B252" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C252" s="25" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="D252" s="25" t="s">
         <v>28</v>
@@ -9873,15 +10188,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="253" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A253" s="25">
         <v>252</v>
       </c>
       <c r="B253" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C253" s="25" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
       <c r="D253" s="25" t="s">
         <v>33</v>
@@ -9898,15 +10213,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="254" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A254" s="25">
         <v>253</v>
       </c>
       <c r="B254" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C254" s="25" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
       <c r="D254" s="25" t="s">
         <v>105</v>
@@ -9923,15 +10238,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="255" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A255" s="25">
         <v>254</v>
       </c>
       <c r="B255" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C255" s="25" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="D255" s="25" t="s">
         <v>33</v>
@@ -9947,16 +10262,19 @@
         <f t="array" ref="N255">SECTION_NAME(B255)</f>
         <v>potential-crd-response-types</v>
       </c>
-    </row>
-    <row r="256" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="P255" s="27" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="256" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A256" s="25">
         <v>255</v>
       </c>
       <c r="B256" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C256" s="25" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
       <c r="D256" s="25" t="s">
         <v>33</v>
@@ -9972,16 +10290,19 @@
         <f t="array" ref="N256">SECTION_NAME(B256)</f>
         <v>potential-crd-response-types</v>
       </c>
-    </row>
-    <row r="257" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P256" s="27" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="257" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A257" s="25">
         <v>256</v>
       </c>
       <c r="B257" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C257" s="25" t="s">
-        <v>344</v>
+        <v>323</v>
       </c>
       <c r="D257" s="25" t="s">
         <v>50</v>
@@ -9998,15 +10319,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="258" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A258" s="25">
         <v>257</v>
       </c>
       <c r="B258" s="33" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="C258" s="25" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
       <c r="D258" s="25" t="s">
         <v>50</v>
@@ -10023,15 +10344,15 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="259" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A259" s="25">
         <v>258</v>
       </c>
       <c r="B259" s="33" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C259" s="25" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
       <c r="D259" s="25" t="s">
         <v>33</v>
@@ -10048,15 +10369,15 @@
         <v>external-reference</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A260" s="25">
         <v>259</v>
       </c>
       <c r="B260" s="33" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C260" s="25" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="D260" s="25" t="s">
         <v>33</v>
@@ -10073,15 +10394,15 @@
         <v>external-reference</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A261" s="25">
         <v>260</v>
       </c>
       <c r="B261" s="33" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C261" s="25" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="D261" s="25" t="s">
         <v>50</v>
@@ -10098,15 +10419,15 @@
         <v>external-reference</v>
       </c>
     </row>
-    <row r="262" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A262" s="25">
         <v>261</v>
       </c>
       <c r="B262" s="33" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
       <c r="C262" s="25" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
       <c r="D262" s="25" t="s">
         <v>50</v>
@@ -10123,15 +10444,15 @@
         <v>external-reference</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A263" s="25">
         <v>262</v>
       </c>
       <c r="B263" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C263" s="25" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
       <c r="D263" s="25" t="s">
         <v>33</v>
@@ -10148,15 +10469,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A264" s="25">
         <v>263</v>
       </c>
       <c r="B264" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C264" s="25" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
       <c r="D264" s="25" t="s">
         <v>33</v>
@@ -10172,16 +10493,19 @@
         <f t="array" ref="N264">SECTION_NAME(B264)</f>
         <v>coverage-information</v>
       </c>
-    </row>
-    <row r="265" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P264" s="27" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="265" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A265" s="25">
         <v>264</v>
       </c>
       <c r="B265" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C265" s="25" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
       <c r="D265" s="25" t="s">
         <v>33</v>
@@ -10198,15 +10522,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="266" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A266" s="25">
         <v>265</v>
       </c>
       <c r="B266" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C266" s="25" t="s">
-        <v>355</v>
+        <v>334</v>
       </c>
       <c r="D266" s="25" t="s">
         <v>33</v>
@@ -10223,15 +10547,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="267" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A267" s="25">
         <v>266</v>
       </c>
       <c r="B267" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C267" s="25" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="D267" s="25" t="s">
         <v>28</v>
@@ -10248,15 +10572,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="268" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A268" s="25">
         <v>267</v>
       </c>
       <c r="B268" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C268" s="25" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="D268" s="25" t="s">
         <v>157</v>
@@ -10273,15 +10597,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="269" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A269" s="25">
         <v>268</v>
       </c>
       <c r="B269" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C269" s="25" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
       <c r="D269" s="25" t="s">
         <v>50</v>
@@ -10298,15 +10622,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="270" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A270" s="25">
         <v>269</v>
       </c>
       <c r="B270" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C270" s="25" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
       <c r="D270" s="25" t="s">
         <v>50</v>
@@ -10323,15 +10647,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="271" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A271" s="25">
         <v>270</v>
       </c>
       <c r="B271" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C271" s="25" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="D271" s="25" t="s">
         <v>50</v>
@@ -10348,15 +10672,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A272" s="25">
         <v>271</v>
       </c>
       <c r="B272" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C272" s="25" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
       <c r="D272" s="25" t="s">
         <v>105</v>
@@ -10373,15 +10697,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="273" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A273" s="25">
         <v>272</v>
       </c>
       <c r="B273" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C273" s="25" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="D273" s="25" t="s">
         <v>33</v>
@@ -10398,15 +10722,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="274" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A274" s="25">
         <v>273</v>
       </c>
       <c r="B274" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C274" s="25" t="s">
-        <v>363</v>
+        <v>342</v>
       </c>
       <c r="D274" s="25" t="s">
         <v>33</v>
@@ -10423,15 +10747,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A275" s="25">
         <v>274</v>
       </c>
       <c r="B275" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C275" s="25" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
       <c r="D275" s="25" t="s">
         <v>33</v>
@@ -10448,15 +10772,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="276" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A276" s="25">
         <v>275</v>
       </c>
       <c r="B276" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C276" s="25" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
       <c r="D276" s="25" t="s">
         <v>33</v>
@@ -10473,15 +10797,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="277" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A277" s="25">
         <v>276</v>
       </c>
       <c r="B277" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C277" s="25" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="D277" s="25" t="s">
         <v>33</v>
@@ -10498,15 +10822,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="278" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A278" s="25">
         <v>277</v>
       </c>
       <c r="B278" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C278" s="25" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
       <c r="D278" s="25" t="s">
         <v>33</v>
@@ -10523,15 +10847,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A279" s="25">
         <v>278</v>
       </c>
       <c r="B279" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C279" s="25" t="s">
-        <v>368</v>
+        <v>347</v>
       </c>
       <c r="D279" s="25" t="s">
         <v>33</v>
@@ -10547,16 +10871,19 @@
         <f t="array" ref="N279">SECTION_NAME(B279)</f>
         <v>coverage-information</v>
       </c>
-    </row>
-    <row r="280" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P279" s="27" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A280" s="25">
         <v>279</v>
       </c>
       <c r="B280" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C280" s="25" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="D280" s="25" t="s">
         <v>33</v>
@@ -10573,15 +10900,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="281" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A281" s="25">
         <v>280</v>
       </c>
       <c r="B281" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C281" s="25" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="D281" s="25" t="s">
         <v>33</v>
@@ -10597,16 +10924,19 @@
         <f t="array" ref="N281">SECTION_NAME(B281)</f>
         <v>coverage-information</v>
       </c>
-    </row>
-    <row r="282" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="P281" s="27" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="282" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A282" s="25">
         <v>281</v>
       </c>
       <c r="B282" s="33" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="C282" s="25" t="s">
-        <v>371</v>
+        <v>350</v>
       </c>
       <c r="D282" s="25" t="s">
         <v>28</v>
@@ -10623,15 +10953,15 @@
         <v>coverage-information</v>
       </c>
     </row>
-    <row r="283" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A283" s="25">
         <v>282</v>
       </c>
       <c r="B283" s="33" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C283" s="25" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="D283" s="25" t="s">
         <v>50</v>
@@ -10648,15 +10978,15 @@
         <v>propose-alternate-request</v>
       </c>
     </row>
-    <row r="284" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A284" s="25">
         <v>283</v>
       </c>
       <c r="B284" s="33" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C284" s="25" t="s">
-        <v>374</v>
+        <v>353</v>
       </c>
       <c r="D284" s="25" t="s">
         <v>50</v>
@@ -10673,15 +11003,15 @@
         <v>propose-alternate-request</v>
       </c>
     </row>
-    <row r="285" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A285" s="25">
         <v>284</v>
       </c>
       <c r="B285" s="33" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C285" s="25" t="s">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="D285" s="25" t="s">
         <v>33</v>
@@ -10697,16 +11027,19 @@
         <f t="array" ref="N285">SECTION_NAME(B285)</f>
         <v>propose-alternate-request</v>
       </c>
-    </row>
-    <row r="286" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+      <c r="P285" s="27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" ht="153" x14ac:dyDescent="0.2">
       <c r="A286" s="25">
         <v>285</v>
       </c>
       <c r="B286" s="33" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C286" s="25" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
       <c r="D286" s="25" t="s">
         <v>33</v>
@@ -10722,16 +11055,19 @@
         <f t="array" ref="N286">SECTION_NAME(B286)</f>
         <v>propose-alternate-request</v>
       </c>
-    </row>
-    <row r="287" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="P286" s="27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A287" s="25">
         <v>286</v>
       </c>
       <c r="B287" s="33" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C287" s="25" t="s">
-        <v>377</v>
+        <v>356</v>
       </c>
       <c r="D287" s="25" t="s">
         <v>33</v>
@@ -10747,16 +11083,19 @@
         <f t="array" ref="N287">SECTION_NAME(B287)</f>
         <v>propose-alternate-request</v>
       </c>
-    </row>
-    <row r="288" spans="1:14" ht="187" x14ac:dyDescent="0.2">
+      <c r="P287" s="27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" ht="187" x14ac:dyDescent="0.2">
       <c r="A288" s="25">
         <v>287</v>
       </c>
       <c r="B288" s="33" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C288" s="25" t="s">
-        <v>378</v>
+        <v>357</v>
       </c>
       <c r="D288" s="25" t="s">
         <v>33</v>
@@ -10772,16 +11111,19 @@
         <f t="array" ref="N288">SECTION_NAME(B288)</f>
         <v>propose-alternate-request</v>
       </c>
-    </row>
-    <row r="289" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="P288" s="27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="289" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A289" s="25">
         <v>288</v>
       </c>
       <c r="B289" s="33" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C289" s="25" t="s">
-        <v>379</v>
+        <v>358</v>
       </c>
       <c r="D289" s="25" t="s">
         <v>33</v>
@@ -10797,16 +11139,19 @@
         <f t="array" ref="N289">SECTION_NAME(B289)</f>
         <v>propose-alternate-request</v>
       </c>
-    </row>
-    <row r="290" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="P289" s="27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="290" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A290" s="25">
         <v>289</v>
       </c>
       <c r="B290" s="33" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C290" s="25" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="D290" s="25" t="s">
         <v>33</v>
@@ -10822,16 +11167,19 @@
         <f t="array" ref="N290">SECTION_NAME(B290)</f>
         <v>propose-alternate-request</v>
       </c>
-    </row>
-    <row r="291" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="P290" s="27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="291" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A291" s="25">
         <v>290</v>
       </c>
       <c r="B291" s="33" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C291" s="25" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
       <c r="D291" s="25" t="s">
         <v>33</v>
@@ -10847,16 +11195,19 @@
         <f t="array" ref="N291">SECTION_NAME(B291)</f>
         <v>propose-alternate-request</v>
       </c>
-    </row>
-    <row r="292" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+      <c r="P291" s="27" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="292" spans="1:16" ht="153" x14ac:dyDescent="0.2">
       <c r="A292" s="25">
         <v>291</v>
       </c>
       <c r="B292" s="33" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="C292" s="25" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
       <c r="D292" s="25" t="s">
         <v>33</v>
@@ -10868,16 +11219,19 @@
         <f t="array" ref="N292">SECTION_NAME(B292)</f>
         <v>identify-additional-orders-as-companionsprerequisites-for-current-order</v>
       </c>
-    </row>
-    <row r="293" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+      <c r="P292" s="27" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="293" spans="1:16" ht="153" x14ac:dyDescent="0.2">
       <c r="A293" s="25">
         <v>292</v>
       </c>
       <c r="B293" s="33" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="C293" s="25" t="s">
-        <v>384</v>
+        <v>363</v>
       </c>
       <c r="D293" s="25" t="s">
         <v>33</v>
@@ -10889,16 +11243,19 @@
         <f t="array" ref="N293">SECTION_NAME(B293)</f>
         <v>identify-additional-orders-as-companionsprerequisites-for-current-order</v>
       </c>
-    </row>
-    <row r="294" spans="1:14" ht="170" x14ac:dyDescent="0.2">
+      <c r="P293" s="27" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="294" spans="1:16" ht="170" x14ac:dyDescent="0.2">
       <c r="A294" s="25">
         <v>293</v>
       </c>
       <c r="B294" s="33" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="C294" s="25" t="s">
-        <v>385</v>
+        <v>364</v>
       </c>
       <c r="D294" s="25" t="s">
         <v>33</v>
@@ -10910,16 +11267,19 @@
         <f t="array" ref="N294">SECTION_NAME(B294)</f>
         <v>identify-additional-orders-as-companionsprerequisites-for-current-order</v>
       </c>
-    </row>
-    <row r="295" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+      <c r="P294" s="27" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="295" spans="1:16" ht="119" x14ac:dyDescent="0.2">
       <c r="A295" s="25">
         <v>294</v>
       </c>
       <c r="B295" s="33" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="C295" s="25" t="s">
-        <v>386</v>
+        <v>365</v>
       </c>
       <c r="D295" s="25" t="s">
         <v>33</v>
@@ -10931,16 +11291,19 @@
         <f t="array" ref="N295">SECTION_NAME(B295)</f>
         <v>identify-additional-orders-as-companionsprerequisites-for-current-order</v>
       </c>
-    </row>
-    <row r="296" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="P295" s="27" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="296" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A296" s="25">
         <v>295</v>
       </c>
       <c r="B296" s="33" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="C296" s="25" t="s">
-        <v>387</v>
+        <v>366</v>
       </c>
       <c r="D296" s="25" t="s">
         <v>33</v>
@@ -10952,16 +11315,19 @@
         <f t="array" ref="N296">SECTION_NAME(B296)</f>
         <v>identify-additional-orders-as-companionsprerequisites-for-current-order</v>
       </c>
-    </row>
-    <row r="297" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P296" s="27" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="297" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A297" s="25">
         <v>296</v>
       </c>
       <c r="B297" s="33" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="C297" s="25" t="s">
-        <v>389</v>
+        <v>368</v>
       </c>
       <c r="D297" s="25" t="s">
         <v>28</v>
@@ -10970,15 +11336,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="298" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A298" s="25">
         <v>297</v>
       </c>
       <c r="B298" s="33" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="C298" s="25" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="D298" s="25" t="s">
         <v>33</v>
@@ -10994,16 +11360,19 @@
         <f t="array" ref="N298">SECTION_NAME(B298)</f>
         <v>request-form-completion</v>
       </c>
-    </row>
-    <row r="299" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="P298" s="27" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="299" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A299" s="25">
         <v>298</v>
       </c>
       <c r="B299" s="33" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="C299" s="25" t="s">
-        <v>391</v>
+        <v>370</v>
       </c>
       <c r="D299" s="25" t="s">
         <v>50</v>
@@ -11020,15 +11389,15 @@
         <v>request-form-completion</v>
       </c>
     </row>
-    <row r="300" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A300" s="25">
         <v>299</v>
       </c>
       <c r="B300" s="33" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="C300" s="25" t="s">
-        <v>392</v>
+        <v>371</v>
       </c>
       <c r="D300" s="25" t="s">
         <v>33</v>
@@ -11045,15 +11414,15 @@
         <v>request-form-completion</v>
       </c>
     </row>
-    <row r="301" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:16" ht="153" x14ac:dyDescent="0.2">
       <c r="A301" s="25">
         <v>300</v>
       </c>
       <c r="B301" s="33" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="C301" s="25" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="D301" s="25" t="s">
         <v>50</v>
@@ -11070,15 +11439,15 @@
         <v>request-form-completion</v>
       </c>
     </row>
-    <row r="302" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A302" s="25">
         <v>301</v>
       </c>
       <c r="B302" s="33" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="C302" s="25" t="s">
-        <v>394</v>
+        <v>373</v>
       </c>
       <c r="D302" s="25" t="s">
         <v>50</v>
@@ -11095,15 +11464,15 @@
         <v>request-form-completion</v>
       </c>
     </row>
-    <row r="303" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A303" s="25">
         <v>302</v>
       </c>
       <c r="B303" s="33" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="C303" s="25" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
       <c r="D303" s="25" t="s">
         <v>28</v>
@@ -11120,15 +11489,15 @@
         <v>create-or-update-coverage-information</v>
       </c>
     </row>
-    <row r="304" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A304" s="25">
         <v>303</v>
       </c>
       <c r="B304" s="33" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="C304" s="25" t="s">
-        <v>397</v>
+        <v>376</v>
       </c>
       <c r="D304" s="25" t="s">
         <v>33</v>
@@ -11144,16 +11513,19 @@
         <f t="array" ref="N304">SECTION_NAME(B304)</f>
         <v>create-or-update-coverage-information</v>
       </c>
-    </row>
-    <row r="305" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="P304" s="27" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="305" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A305" s="25">
         <v>304</v>
       </c>
       <c r="B305" s="33" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="C305" s="25" t="s">
-        <v>398</v>
+        <v>377</v>
       </c>
       <c r="D305" s="25" t="s">
         <v>28</v>
@@ -11170,15 +11542,15 @@
         <v>create-or-update-coverage-information</v>
       </c>
     </row>
-    <row r="306" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A306" s="25">
         <v>305</v>
       </c>
       <c r="B306" s="33" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="C306" s="25" t="s">
-        <v>399</v>
+        <v>378</v>
       </c>
       <c r="D306" s="25" t="s">
         <v>157</v>
@@ -11195,15 +11567,15 @@
         <v>create-or-update-coverage-information</v>
       </c>
     </row>
-    <row r="307" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A307" s="25">
         <v>306</v>
       </c>
       <c r="B307" s="33" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="C307" s="25" t="s">
-        <v>400</v>
+        <v>379</v>
       </c>
       <c r="D307" s="25" t="s">
         <v>33</v>
@@ -11220,15 +11592,15 @@
         <v>create-or-update-coverage-information</v>
       </c>
     </row>
-    <row r="308" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A308" s="25">
         <v>307</v>
       </c>
       <c r="B308" s="33" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="C308" s="25" t="s">
-        <v>402</v>
+        <v>381</v>
       </c>
       <c r="D308" s="25" t="s">
         <v>28</v>
@@ -11245,15 +11617,15 @@
         <v>launch-smart-application</v>
       </c>
     </row>
-    <row r="309" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A309" s="25">
         <v>308</v>
       </c>
       <c r="B309" s="33" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="C309" s="25" t="s">
-        <v>404</v>
+        <v>383</v>
       </c>
       <c r="D309" s="25" t="s">
         <v>33</v>
@@ -11269,16 +11641,19 @@
         <f t="array" ref="N309">SECTION_NAME(B309)</f>
         <v>suppressing-guidance</v>
       </c>
-    </row>
-    <row r="310" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="P309" s="27" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="310" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A310" s="25">
         <v>309</v>
       </c>
       <c r="B310" s="33" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="C310" s="25" t="s">
-        <v>406</v>
+        <v>385</v>
       </c>
       <c r="D310" s="25" t="s">
         <v>50</v>
@@ -11295,15 +11670,15 @@
         <v>impact-on-payer-processes</v>
       </c>
     </row>
-    <row r="311" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:16" ht="136" x14ac:dyDescent="0.2">
       <c r="A311" s="25">
         <v>310</v>
       </c>
       <c r="B311" s="33" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="C311" s="25" t="s">
-        <v>407</v>
+        <v>386</v>
       </c>
       <c r="D311" s="25" t="s">
         <v>50</v>
@@ -11320,15 +11695,15 @@
         <v>impact-on-payer-processes</v>
       </c>
     </row>
-    <row r="312" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:16" ht="68" x14ac:dyDescent="0.2">
       <c r="A312" s="25">
         <v>311</v>
       </c>
       <c r="B312" s="33" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="C312" s="25" t="s">
-        <v>408</v>
+        <v>387</v>
       </c>
       <c r="D312" s="25" t="s">
         <v>28</v>
@@ -11345,10 +11720,10 @@
         <v>impact-on-payer-processes</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B313" s="33"/>
     </row>
-    <row r="314" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B314" s="33"/>
       <c r="M314" s="30" t="str" cm="1">
         <f t="array" ref="M314">PAGE_NAME(B314)</f>
@@ -11359,7 +11734,7 @@
         <v/>
       </c>
     </row>
-    <row r="315" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B315" s="33"/>
       <c r="M315" s="30" t="str" cm="1">
         <f t="array" ref="M315">PAGE_NAME(B315)</f>
@@ -11370,7 +11745,7 @@
         <v/>
       </c>
     </row>
-    <row r="316" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B316" s="33"/>
       <c r="M316" s="30" t="str" cm="1">
         <f t="array" ref="M316">PAGE_NAME(B316)</f>
@@ -11381,7 +11756,7 @@
         <v/>
       </c>
     </row>
-    <row r="317" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B317" s="33"/>
       <c r="M317" s="30" t="str" cm="1">
         <f t="array" ref="M317">PAGE_NAME(B317)</f>
@@ -11392,7 +11767,7 @@
         <v/>
       </c>
     </row>
-    <row r="318" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B318" s="33"/>
       <c r="M318" s="30" t="str" cm="1">
         <f t="array" ref="M318">PAGE_NAME(B318)</f>
@@ -11403,7 +11778,7 @@
         <v/>
       </c>
     </row>
-    <row r="319" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B319" s="33"/>
       <c r="M319" s="30" t="str" cm="1">
         <f t="array" ref="M319">PAGE_NAME(B319)</f>
@@ -11414,7 +11789,7 @@
         <v/>
       </c>
     </row>
-    <row r="320" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B320" s="33"/>
       <c r="M320" s="30" t="str" cm="1">
         <f t="array" ref="M320">PAGE_NAME(B320)</f>
@@ -12880,83 +13255,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
-        <v>444</v>
-      </c>
-      <c r="B1" s="40"/>
+      <c r="A1" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="B1" s="48"/>
     </row>
     <row r="2" spans="1:2" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>409</v>
+        <v>388</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>410</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>411</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -12984,19 +13359,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -13004,13 +13379,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="D2" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
       <c r="E2" s="23">
         <v>45583</v>
@@ -13034,13 +13409,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>433</v>
+        <v>412</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -13054,10 +13429,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="D2" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -13068,10 +13443,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>436</v>
+        <v>415</v>
       </c>
       <c r="D3" t="s">
-        <v>437</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -13079,7 +13454,7 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -13103,15 +13478,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
@@ -13122,6 +13488,15 @@
     <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13379,14 +13754,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -13400,6 +13767,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
deprecate CRD requirement 254
</commit_message>
<xml_diff>
--- a/lib/davinci_crd_test_kit/requirements/hl7.fhir.us.davinci-crd_2.0.1_requirements.xlsx
+++ b/lib/davinci_crd_test_kit/requirements/hl7.fhir.us.davinci-crd_2.0.1_requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlnaden/GlenViewAssociates/Inferno/source/davinci-crd-test-kit/lib/davinci_crd_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094A3B58-42DD-5049-B4B7-07D172D22508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE9B761-2B41-F642-9077-0513480C27A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="760" windowWidth="34260" windowHeight="21260" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="2200" yWindow="3000" windowWidth="34260" windowHeight="21260" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="489">
   <si>
     <r>
       <rPr>
@@ -3096,6 +3096,9 @@
       </rPr>
       <t>](https://hl7.org/fhir/us/davinci-crd/STU2/StructureDefinition-profile-appointment.html)</t>
     </r>
+  </si>
+  <si>
+    <t>Deprecated because this is an explanation of what implementers need to do internally to accomplish requirements, for example, adding coverage-information extensions to provided orders (See equirements 278 and 280)</t>
   </si>
 </sst>
 </file>
@@ -4022,10 +4025,10 @@
   <dimension ref="A1:AE434"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="J176" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="R250" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C181" sqref="C178:C181"/>
+      <selection pane="bottomRight" activeCell="T256" sqref="T256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9951,7 +9954,7 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="241" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A241" s="25">
         <v>240</v>
       </c>
@@ -9976,7 +9979,7 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="242" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A242" s="25">
         <v>241</v>
       </c>
@@ -10001,7 +10004,7 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="243" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A243" s="25">
         <v>242</v>
       </c>
@@ -10026,7 +10029,7 @@
         <v>cards-profiles</v>
       </c>
     </row>
-    <row r="244" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A244" s="25">
         <v>243</v>
       </c>
@@ -10054,7 +10057,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="245" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A245" s="25">
         <v>244</v>
       </c>
@@ -10082,7 +10085,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="246" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A246" s="25">
         <v>245</v>
       </c>
@@ -10110,7 +10113,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="247" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A247" s="25">
         <v>246</v>
       </c>
@@ -10135,7 +10138,7 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="248" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A248" s="25">
         <v>247</v>
       </c>
@@ -10160,7 +10163,7 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="249" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A249" s="25">
         <v>248</v>
       </c>
@@ -10185,7 +10188,7 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="250" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A250" s="25">
         <v>249</v>
       </c>
@@ -10210,7 +10213,7 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="251" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A251" s="25">
         <v>250</v>
       </c>
@@ -10235,7 +10238,7 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="252" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A252" s="25">
         <v>251</v>
       </c>
@@ -10260,7 +10263,7 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="253" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A253" s="25">
         <v>252</v>
       </c>
@@ -10285,7 +10288,7 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="254" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A254" s="25">
         <v>253</v>
       </c>
@@ -10310,7 +10313,7 @@
         <v>potential-crd-response-types</v>
       </c>
     </row>
-    <row r="255" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A255" s="25">
         <v>254</v>
       </c>
@@ -10321,7 +10324,7 @@
         <v>310</v>
       </c>
       <c r="D255" s="25" t="s">
-        <v>33</v>
+        <v>206</v>
       </c>
       <c r="E255" s="25" t="s">
         <v>34</v>
@@ -10337,8 +10340,11 @@
       <c r="P255" s="27" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="256" spans="1:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="T255" s="27" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="256" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A256" s="25">
         <v>255</v>
       </c>

</xml_diff>

<commit_message>
add client capability statement requirements
</commit_message>
<xml_diff>
--- a/lib/davinci_crd_test_kit/requirements/hl7.fhir.us.davinci-crd_2.0.1_requirements.xlsx
+++ b/lib/davinci_crd_test_kit/requirements/hl7.fhir.us.davinci-crd_2.0.1_requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlnaden/GlenViewAssociates/Inferno/source/davinci-crd-test-kit/lib/davinci_crd_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE9B761-2B41-F642-9077-0513480C27A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2004C8-3BAD-084E-B65B-BA41D128F7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="3000" windowWidth="34260" windowHeight="21260" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="160" yWindow="920" windowWidth="34260" windowHeight="21260" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="494">
   <si>
     <r>
       <rPr>
@@ -3099,6 +3099,21 @@
   </si>
   <si>
     <t>Deprecated because this is an explanation of what implementers need to do internally to accomplish requirements, for example, adding coverage-information extensions to provided orders (See equirements 278 and 280)</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/us/davinci-crd/STU2/CapabilityStatement-crd-client.html</t>
+  </si>
+  <si>
+    <t>the CRD Client SHALL support all ‘SHOULD’ ‘read’ and ‘search’ capabilities listed below for resources referenced in supported hooks and order types if it does not support returning the associated resources as part of CDS Hooks pre-fetch.</t>
+  </si>
+  <si>
+    <t>The CRD Client SHALL also support ‘update’ functionality for all resources listed below where the client allows invoking hooks based on the resource.</t>
+  </si>
+  <si>
+    <t>Implementations SHALL meet the general security requirements documented in the [HRex implementation guide](http://hl7.org/fhir/us/davinci-hrex/STU1/security.html)</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/us/davinci-crd/STU2/CapabilityStatement-crd-client.html#mode1</t>
   </si>
 </sst>
 </file>
@@ -4025,10 +4040,10 @@
   <dimension ref="A1:AE434"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="R250" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F310" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T256" sqref="T256"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7324,7 +7339,7 @@
         <v>hook-configuration-extension</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:20" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A133" s="25">
         <v>132</v>
       </c>
@@ -11798,29 +11813,71 @@
         <v>impact-on-payer-processes</v>
       </c>
     </row>
-    <row r="313" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B313" s="33"/>
-    </row>
-    <row r="314" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B314" s="33"/>
+    <row r="313" spans="1:16" ht="68" x14ac:dyDescent="0.2">
+      <c r="A313" s="25">
+        <v>312</v>
+      </c>
+      <c r="B313" s="33" t="s">
+        <v>489</v>
+      </c>
+      <c r="C313" s="25" t="s">
+        <v>490</v>
+      </c>
+      <c r="D313" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E313" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="314" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A314" s="25">
+        <v>313</v>
+      </c>
+      <c r="B314" s="33" t="s">
+        <v>489</v>
+      </c>
+      <c r="C314" s="25" t="s">
+        <v>491</v>
+      </c>
+      <c r="D314" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E314" s="25" t="s">
+        <v>34</v>
+      </c>
       <c r="M314" s="30" t="str" cm="1">
         <f t="array" ref="M314">PAGE_NAME(B314)</f>
-        <v/>
+        <v>CapabilityStatement-crd-client</v>
       </c>
       <c r="N314" s="30" t="str" cm="1">
         <f t="array" ref="N314">SECTION_NAME(B314)</f>
         <v/>
       </c>
     </row>
-    <row r="315" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B315" s="33"/>
+    <row r="315" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A315" s="25">
+        <v>314</v>
+      </c>
+      <c r="B315" s="33" t="s">
+        <v>493</v>
+      </c>
+      <c r="C315" s="25" t="s">
+        <v>492</v>
+      </c>
+      <c r="D315" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E315" s="25" t="s">
+        <v>34</v>
+      </c>
       <c r="M315" s="30" t="str" cm="1">
         <f t="array" ref="M315">PAGE_NAME(B315)</f>
-        <v/>
+        <v>CapabilityStatement-crd-client</v>
       </c>
       <c r="N315" s="30" t="str" cm="1">
         <f t="array" ref="N315">SECTION_NAME(B315)</f>
-        <v/>
+        <v>mode1</v>
       </c>
     </row>
     <row r="316" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -13289,6 +13346,9 @@
     <hyperlink ref="B43" r:id="rId259" location="additional-data-retrieval" xr:uid="{4CA5E12F-5D9B-4E70-BFE0-23078A77DAD2}"/>
     <hyperlink ref="B61" r:id="rId260" location="query-notes" xr:uid="{F352642C-5E42-44B7-A229-709C7B04AFA5}"/>
     <hyperlink ref="B35" r:id="rId261" location="enabling-a-crd-server" xr:uid="{29492AB6-A2B3-4D6D-AE1A-D0642733CC57}"/>
+    <hyperlink ref="B313" r:id="rId262" xr:uid="{5A7044E4-ECC6-8346-910D-AA03F675DEC7}"/>
+    <hyperlink ref="B314" r:id="rId263" xr:uid="{2FA4B1FA-85FD-AD4D-BEA5-6604BC45F12B}"/>
+    <hyperlink ref="B315" r:id="rId264" location="mode1" xr:uid="{F4E24FAE-9A70-494A-B2FE-AAD9593C3236}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -13304,7 +13364,7 @@
           <x14:formula1>
             <xm:f>'Column Data'!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D298:D1048576 D2:D296</xm:sqref>
+          <xm:sqref>D2:D296 D298:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4FB27A2-804E-CB49-B85C-BBEE0C688B4F}">
           <x14:formula1>
@@ -13569,15 +13629,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -13831,6 +13882,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
   <ds:schemaRefs>
@@ -13850,14 +13910,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45EEC221-F5CD-4DEF-B390-EE14E23A8785}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13875,4 +13927,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add access token requirement
</commit_message>
<xml_diff>
--- a/lib/davinci_crd_test_kit/requirements/hl7.fhir.us.davinci-crd_2.0.1_requirements.xlsx
+++ b/lib/davinci_crd_test_kit/requirements/hl7.fhir.us.davinci-crd_2.0.1_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlnaden/GlenViewAssociates/Inferno/source/davinci-crd-test-kit/lib/davinci_crd_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902D4EC5-DE23-B445-BB2D-4C749561019A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F22370C-3EBF-A84B-A177-C594769D23FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1578" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="505">
   <si>
     <r>
       <rPr>
@@ -3148,6 +3148,9 @@
 - Coverage search by status not required by US Core
 - Encounter search by location (with patient) required by US Core starting in US Core 5
 - PractitionerRole search by organization and id not required by US Core</t>
+  </si>
+  <si>
+    <t>When a CRD client invokes a CRD server via CDS Hooks, it will provide an access token that allows the CRD server to retrieve additional patient information.</t>
   </si>
 </sst>
 </file>
@@ -4074,10 +4077,10 @@
   <dimension ref="A1:AE433"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F311" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="J320" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T316" sqref="T316"/>
+      <selection pane="bottomRight" activeCell="P324" sqref="P324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12156,15 +12159,32 @@
         <v>440</v>
       </c>
     </row>
-    <row r="324" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B324" s="33"/>
+    <row r="324" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A324" s="25">
+        <v>323</v>
+      </c>
+      <c r="B324" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C324" s="25" t="s">
+        <v>504</v>
+      </c>
+      <c r="D324" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E324" s="25" t="s">
+        <v>34</v>
+      </c>
       <c r="M324" s="30" t="str" cm="1">
         <f t="array" ref="M324">PAGE_NAME(B324)</f>
-        <v/>
+        <v>foundation</v>
       </c>
       <c r="N324" s="30" t="str" cm="1">
         <f t="array" ref="N324">SECTION_NAME(B324)</f>
-        <v/>
+        <v>crd-access-tokens</v>
+      </c>
+      <c r="P324" s="27" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="325" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -13534,6 +13554,7 @@
     <hyperlink ref="B321" r:id="rId270" xr:uid="{97C55971-E2C3-7244-81CA-BD37FB24BFA3}"/>
     <hyperlink ref="B322" r:id="rId271" xr:uid="{43BF7D95-9CEA-1040-9742-52552CCADCCF}"/>
     <hyperlink ref="B323" r:id="rId272" xr:uid="{18B2CDF4-D33C-B14E-A306-E6D686E42A3C}"/>
+    <hyperlink ref="B324" r:id="rId273" location="crd-access-tokens" xr:uid="{B501E1B5-4CEF-F54F-B165-9093BF92BC2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -13801,16 +13822,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14068,28 +14085,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14115,9 +14126,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>